<commit_message>
feat: add script to to do enrichment analysis
</commit_message>
<xml_diff>
--- a/ComplementaryData/chemicals_info.xlsx
+++ b/ComplementaryData/chemicals_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Documents/GitHub/CellFactory-yeast-GEM/ComplementaryData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xluhon/Documents/GitHub/CellFactory-yeast-GEM/ComplementaryData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB0B87EB-DA3C-7C41-A77A-6A4C7FD389CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB3BDBE-D51C-414F-9FDC-05CC55A4C422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="1340" yWindow="660" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="chemicals_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="502">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,9 @@
     <t>C03044</t>
   </si>
   <si>
+    <t>90.121</t>
+  </si>
+  <si>
     <t>native</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>C05853</t>
   </si>
   <si>
+    <t>122.1644</t>
+  </si>
+  <si>
     <t>ec2-phenylethanol.mat</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
     <t>C00116</t>
   </si>
   <si>
+    <t>92.09382</t>
+  </si>
+  <si>
     <t>ecGlycerol.mat</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
     <t>C07328</t>
   </si>
   <si>
+    <t>88.14818</t>
+  </si>
+  <si>
     <t>ec3-methylbutanol.mat</t>
   </si>
   <si>
@@ -109,6 +121,9 @@
     <t>C14710</t>
   </si>
   <si>
+    <t>74.1216</t>
+  </si>
+  <si>
     <t>ecIsobutanol.mat</t>
   </si>
   <si>
@@ -121,6 +136,9 @@
     <t>C00114</t>
   </si>
   <si>
+    <t>104.1708</t>
+  </si>
+  <si>
     <t>alkaloid</t>
   </si>
   <si>
@@ -136,6 +154,9 @@
     <t>C00262</t>
   </si>
   <si>
+    <t>136.11162</t>
+  </si>
+  <si>
     <t>ecHypoxanthine.mat</t>
   </si>
   <si>
@@ -148,6 +169,9 @@
     <t>C00385</t>
   </si>
   <si>
+    <t>152.11102</t>
+  </si>
+  <si>
     <t>ecXanthine.mat</t>
   </si>
   <si>
@@ -160,6 +184,9 @@
     <t>C00051</t>
   </si>
   <si>
+    <t>307.32</t>
+  </si>
+  <si>
     <t>amino acid</t>
   </si>
   <si>
@@ -175,6 +202,9 @@
     <t>C00041</t>
   </si>
   <si>
+    <t>89.09322</t>
+  </si>
+  <si>
     <t>ecAlanine.mat</t>
   </si>
   <si>
@@ -187,6 +217,9 @@
     <t>C00062</t>
   </si>
   <si>
+    <t>174.201</t>
+  </si>
+  <si>
     <t>ecArginine.mat</t>
   </si>
   <si>
@@ -199,6 +232,9 @@
     <t>C00152</t>
   </si>
   <si>
+    <t>132.118001</t>
+  </si>
+  <si>
     <t>ecAsparagine.mat</t>
   </si>
   <si>
@@ -211,6 +247,9 @@
     <t>C00049</t>
   </si>
   <si>
+    <t>133.1027</t>
+  </si>
+  <si>
     <t>ecAspartate.mat</t>
   </si>
   <si>
@@ -223,6 +262,9 @@
     <t>C00327</t>
   </si>
   <si>
+    <t>175.18584</t>
+  </si>
+  <si>
     <t>ecCitrulline.mat</t>
   </si>
   <si>
@@ -235,6 +277,9 @@
     <t>C00097</t>
   </si>
   <si>
+    <t>121.158</t>
+  </si>
+  <si>
     <t>ecCysteine.mat</t>
   </si>
   <si>
@@ -247,6 +292,9 @@
     <t>C00025</t>
   </si>
   <si>
+    <t>146.12136</t>
+  </si>
+  <si>
     <t>ecGlutamate.mat</t>
   </si>
   <si>
@@ -259,6 +307,9 @@
     <t>C00064</t>
   </si>
   <si>
+    <t>146.14458</t>
+  </si>
+  <si>
     <t>ecGlutamine.mat</t>
   </si>
   <si>
@@ -271,6 +322,9 @@
     <t>C00037</t>
   </si>
   <si>
+    <t>75.06664</t>
+  </si>
+  <si>
     <t>ecGlycine.mat</t>
   </si>
   <si>
@@ -283,6 +337,9 @@
     <t>C00135</t>
   </si>
   <si>
+    <t>155.15468</t>
+  </si>
+  <si>
     <t>ecHistidine.mat</t>
   </si>
   <si>
@@ -295,6 +352,9 @@
     <t>C00263</t>
   </si>
   <si>
+    <t>119.1192</t>
+  </si>
+  <si>
     <t>ecHomoserine.mat</t>
   </si>
   <si>
@@ -307,6 +367,9 @@
     <t>C00407</t>
   </si>
   <si>
+    <t>131.175</t>
+  </si>
+  <si>
     <t>ecIsoleucine.mat</t>
   </si>
   <si>
@@ -316,6 +379,9 @@
     <t>C00123</t>
   </si>
   <si>
+    <t>131.17296</t>
+  </si>
+  <si>
     <t>ecLeucine.mat</t>
   </si>
   <si>
@@ -328,6 +394,9 @@
     <t>C00047</t>
   </si>
   <si>
+    <t>147.19558</t>
+  </si>
+  <si>
     <t>ecLysine.mat</t>
   </si>
   <si>
@@ -340,6 +409,9 @@
     <t>C00073</t>
   </si>
   <si>
+    <t>149.21238</t>
+  </si>
+  <si>
     <t>ecMethionine.mat</t>
   </si>
   <si>
@@ -352,6 +424,9 @@
     <t>C00079</t>
   </si>
   <si>
+    <t>165.18918</t>
+  </si>
+  <si>
     <t>ecPhenylalanine.mat</t>
   </si>
   <si>
@@ -364,6 +439,9 @@
     <t>C00148</t>
   </si>
   <si>
+    <t>115.1305</t>
+  </si>
+  <si>
     <t>ecProline.mat</t>
   </si>
   <si>
@@ -376,6 +454,9 @@
     <t>C00065</t>
   </si>
   <si>
+    <t>105.09262</t>
+  </si>
+  <si>
     <t>ecSerine.mat</t>
   </si>
   <si>
@@ -397,6 +478,9 @@
     <t>C00078</t>
   </si>
   <si>
+    <t>204.22526</t>
+  </si>
+  <si>
     <t>ecTryptophan.mat</t>
   </si>
   <si>
@@ -409,6 +493,9 @@
     <t>C00082</t>
   </si>
   <si>
+    <t>181.18858</t>
+  </si>
+  <si>
     <t>ecTyrosine.mat</t>
   </si>
   <si>
@@ -421,6 +508,9 @@
     <t>C00183</t>
   </si>
   <si>
+    <t>117.14638</t>
+  </si>
+  <si>
     <t>ecValine.mat</t>
   </si>
   <si>
@@ -433,6 +523,9 @@
     <t>C01602</t>
   </si>
   <si>
+    <t>133.169</t>
+  </si>
+  <si>
     <t>ecOrnithine.mat</t>
   </si>
   <si>
@@ -445,6 +538,9 @@
     <t>C00134</t>
   </si>
   <si>
+    <t>90.1674</t>
+  </si>
+  <si>
     <t>bioamine</t>
   </si>
   <si>
@@ -460,12 +556,18 @@
     <t>C00750</t>
   </si>
   <si>
+    <t>206.372</t>
+  </si>
+  <si>
     <t>ecSpermine.mat</t>
   </si>
   <si>
     <t>Free fatty acids</t>
   </si>
   <si>
+    <t>396.64836</t>
+  </si>
+  <si>
     <t>fatty acids and lipids</t>
   </si>
   <si>
@@ -481,6 +583,9 @@
     <t>C02679</t>
   </si>
   <si>
+    <t>199.31</t>
+  </si>
+  <si>
     <t>ecLaurate.mat</t>
   </si>
   <si>
@@ -493,6 +598,9 @@
     <t>C00712</t>
   </si>
   <si>
+    <t>282.4614</t>
+  </si>
+  <si>
     <t>ecOleate.mat</t>
   </si>
   <si>
@@ -505,6 +613,9 @@
     <t>C08362</t>
   </si>
   <si>
+    <t>253.40026</t>
+  </si>
+  <si>
     <t>ecPalmitoleate.mat</t>
   </si>
   <si>
@@ -517,6 +628,9 @@
     <t>C00042</t>
   </si>
   <si>
+    <t>116.07216</t>
+  </si>
+  <si>
     <t>ecSuc-reTCA.mat</t>
   </si>
   <si>
@@ -529,6 +643,9 @@
     <t>C00422</t>
   </si>
   <si>
+    <t>173.1003</t>
+  </si>
+  <si>
     <t>ectriacylglycerol.mat</t>
   </si>
   <si>
@@ -541,6 +658,9 @@
     <t>C00242</t>
   </si>
   <si>
+    <t>151.126</t>
+  </si>
+  <si>
     <t>nucleic acid</t>
   </si>
   <si>
@@ -556,6 +676,9 @@
     <t>C00214</t>
   </si>
   <si>
+    <t>242.2286</t>
+  </si>
+  <si>
     <t>ecThymidine.mat</t>
   </si>
   <si>
@@ -568,6 +691,9 @@
     <t>C00186</t>
   </si>
   <si>
+    <t>89.07</t>
+  </si>
+  <si>
     <t>organic acid</t>
   </si>
   <si>
@@ -583,6 +709,9 @@
     <t>C00149</t>
   </si>
   <si>
+    <t>132.07156</t>
+  </si>
+  <si>
     <t>ecMalate.mat</t>
   </si>
   <si>
@@ -595,6 +724,9 @@
     <t>C00026</t>
   </si>
   <si>
+    <t>144.08226</t>
+  </si>
+  <si>
     <t>ecOxoglutarate.mat</t>
   </si>
   <si>
@@ -607,6 +739,9 @@
     <t>C00033</t>
   </si>
   <si>
+    <t>60.052</t>
+  </si>
+  <si>
     <t>ecAcetate.mat</t>
   </si>
   <si>
@@ -619,6 +754,9 @@
     <t>C00158</t>
   </si>
   <si>
+    <t>189.0997</t>
+  </si>
+  <si>
     <t>ecCitrate.mat</t>
   </si>
   <si>
@@ -628,6 +766,9 @@
     <t>C00122</t>
   </si>
   <si>
+    <t>116.0722</t>
+  </si>
+  <si>
     <t>ecFumaric_acid.mat</t>
   </si>
   <si>
@@ -640,6 +781,9 @@
     <t>C00160</t>
   </si>
   <si>
+    <t>76.05136</t>
+  </si>
+  <si>
     <t>ecGlycolate.mat</t>
   </si>
   <si>
@@ -652,6 +796,9 @@
     <t>C01585</t>
   </si>
   <si>
+    <t>115.15034</t>
+  </si>
+  <si>
     <t>ecHexanoate.mat</t>
   </si>
   <si>
@@ -664,6 +811,9 @@
     <t>C00022</t>
   </si>
   <si>
+    <t>87.05412</t>
+  </si>
+  <si>
     <t>ecPyruvate.mat</t>
   </si>
   <si>
@@ -676,6 +826,9 @@
     <t>C00084</t>
   </si>
   <si>
+    <t>44.05256</t>
+  </si>
+  <si>
     <t>other</t>
   </si>
   <si>
@@ -691,6 +844,9 @@
     <t>C00086</t>
   </si>
   <si>
+    <t>60.05534</t>
+  </si>
+  <si>
     <t>ecUrea.mat</t>
   </si>
   <si>
@@ -748,6 +904,9 @@
     <t>C07576</t>
   </si>
   <si>
+    <t>284.248101</t>
+  </si>
+  <si>
     <t>ecPsilocybin.mat</t>
   </si>
   <si>
@@ -1286,6 +1445,87 @@
   </si>
   <si>
     <t>ecbeta_Ionone.mat</t>
+  </si>
+  <si>
+    <t>fucosyllactose</t>
+  </si>
+  <si>
+    <t>ec2_fucosyllactose.mat</t>
+  </si>
+  <si>
+    <t>caffeicacid</t>
+  </si>
+  <si>
+    <t>eccaffeic_acid.mat</t>
+  </si>
+  <si>
+    <t>cinnamoyltropine</t>
+  </si>
+  <si>
+    <t>eccinnamoyltropine.mat</t>
+  </si>
+  <si>
+    <t>ergothioneine</t>
+  </si>
+  <si>
+    <t>ecergothioneine.mat</t>
+  </si>
+  <si>
+    <t>glycyrrhetinic_acid</t>
+  </si>
+  <si>
+    <t>ecglycyrrhetinic_acid.mat</t>
+  </si>
+  <si>
+    <t>lycopene</t>
+  </si>
+  <si>
+    <t>eclycopene.mat</t>
+  </si>
+  <si>
+    <t>miltiradiene</t>
+  </si>
+  <si>
+    <t>ecmiltiradiene.mat</t>
+  </si>
+  <si>
+    <t>nootkatone</t>
+  </si>
+  <si>
+    <t>ecnootkatone.mat</t>
+  </si>
+  <si>
+    <t>s-adenosyl-l-methionine</t>
+  </si>
+  <si>
+    <t>ecs-adenosyl-l-methionine.mat</t>
+  </si>
+  <si>
+    <t>squalene</t>
+  </si>
+  <si>
+    <t>ecsqualene.mat</t>
+  </si>
+  <si>
+    <t>ecsuccinate.mat</t>
+  </si>
+  <si>
+    <t>taxadien_5alpha_yl_acetate</t>
+  </si>
+  <si>
+    <t>ectaxadien_5alpha_yl_acetate.mat</t>
+  </si>
+  <si>
+    <t>vitamin_a</t>
+  </si>
+  <si>
+    <t>ecvitamin_a.mat</t>
+  </si>
+  <si>
+    <t>valencene</t>
+  </si>
+  <si>
+    <t>ecvalencene.mat</t>
   </si>
 </sst>
 </file>
@@ -2126,16 +2366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2176,1417 +2413,1417 @@
       <c r="D2">
         <v>16982</v>
       </c>
-      <c r="E2">
-        <v>90.120999999999995</v>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>49000</v>
       </c>
-      <c r="E3">
-        <v>122.1644</v>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>17754</v>
       </c>
-      <c r="E4">
-        <v>92.093819999999994</v>
+      <c r="E4" t="s">
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>15837</v>
       </c>
-      <c r="E5">
-        <v>88.148179999999996</v>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>46645</v>
       </c>
-      <c r="E6">
-        <v>74.121600000000001</v>
+      <c r="E6" t="s">
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>15354</v>
       </c>
-      <c r="E7">
-        <v>104.1708</v>
+      <c r="E7" t="s">
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>17368</v>
       </c>
-      <c r="E8">
-        <v>136.11161999999999</v>
+      <c r="E8" t="s">
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>17712</v>
       </c>
-      <c r="E9">
-        <v>152.11102</v>
+      <c r="E9" t="s">
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>16856</v>
       </c>
-      <c r="E10">
-        <v>307.32</v>
+      <c r="E10" t="s">
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>16977</v>
       </c>
-      <c r="E11">
-        <v>89.093220000000002</v>
+      <c r="E11" t="s">
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>16467</v>
       </c>
-      <c r="E12">
-        <v>174.20099999999999</v>
+      <c r="E12" t="s">
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>17196</v>
       </c>
-      <c r="E13">
-        <v>132.11800099999999</v>
+      <c r="E13" t="s">
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>17053</v>
       </c>
-      <c r="E14">
-        <v>133.1027</v>
+      <c r="E14" t="s">
+        <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D15">
         <v>16349</v>
       </c>
-      <c r="E15">
-        <v>175.18584000000001</v>
+      <c r="E15" t="s">
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D16">
         <v>17561</v>
       </c>
-      <c r="E16">
-        <v>121.158</v>
+      <c r="E16" t="s">
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D17">
         <v>29985</v>
       </c>
-      <c r="E17">
-        <v>146.12136000000001</v>
+      <c r="E17" t="s">
+        <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D18">
         <v>18050</v>
       </c>
-      <c r="E18">
-        <v>146.14457999999999</v>
+      <c r="E18" t="s">
+        <v>95</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D19">
         <v>15428</v>
       </c>
-      <c r="E19">
-        <v>75.066640000000007</v>
+      <c r="E19" t="s">
+        <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D20">
         <v>15971</v>
       </c>
-      <c r="E20">
-        <v>155.15468000000001</v>
+      <c r="E20" t="s">
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D21">
         <v>15699</v>
       </c>
-      <c r="E21">
-        <v>119.11920000000001</v>
+      <c r="E21" t="s">
+        <v>110</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="D22">
         <v>17191</v>
       </c>
-      <c r="E22">
-        <v>131.17500000000001</v>
+      <c r="E22" t="s">
+        <v>115</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D23">
         <v>15603</v>
       </c>
-      <c r="E23">
-        <v>131.17295999999999</v>
+      <c r="E23" t="s">
+        <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D24">
         <v>32551</v>
       </c>
-      <c r="E24">
-        <v>147.19558000000001</v>
+      <c r="E24" t="s">
+        <v>124</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="D25">
         <v>16643</v>
       </c>
-      <c r="E25">
-        <v>149.21238</v>
+      <c r="E25" t="s">
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D26">
         <v>17295</v>
       </c>
-      <c r="E26">
-        <v>165.18917999999999</v>
+      <c r="E26" t="s">
+        <v>134</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H26" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D27">
         <v>17203</v>
       </c>
-      <c r="E27">
-        <v>115.1305</v>
+      <c r="E27" t="s">
+        <v>139</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="D28">
         <v>17115</v>
       </c>
-      <c r="E28">
-        <v>105.09262</v>
+      <c r="E28" t="s">
+        <v>144</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="D29">
         <v>16857</v>
       </c>
-      <c r="E29">
-        <v>119.11920000000001</v>
+      <c r="E29" t="s">
+        <v>110</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D30">
         <v>16828</v>
       </c>
-      <c r="E30">
-        <v>204.22525999999999</v>
+      <c r="E30" t="s">
+        <v>152</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="D31">
         <v>17895</v>
       </c>
-      <c r="E31">
-        <v>181.18858</v>
+      <c r="E31" t="s">
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H31" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="D32">
         <v>16414</v>
       </c>
-      <c r="E32">
-        <v>117.14637999999999</v>
+      <c r="E32" t="s">
+        <v>162</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H32" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="D33">
         <v>46912</v>
       </c>
-      <c r="E33">
-        <v>133.16900000000001</v>
+      <c r="E33" t="s">
+        <v>167</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H33" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="D34">
         <v>326268</v>
       </c>
-      <c r="E34">
-        <v>90.167400000000001</v>
+      <c r="E34" t="s">
+        <v>172</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="H34" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="D35">
         <v>45725</v>
       </c>
-      <c r="E35">
-        <v>206.37200000000001</v>
+      <c r="E35" t="s">
+        <v>178</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="H35" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36">
-        <v>396.64836000000003</v>
+        <v>180</v>
+      </c>
+      <c r="E36" t="s">
+        <v>181</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H36" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="D37">
         <v>18262</v>
       </c>
-      <c r="E37">
-        <v>199.31</v>
+      <c r="E37" t="s">
+        <v>187</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H37" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="D38">
         <v>16196</v>
       </c>
-      <c r="E38">
-        <v>282.46140000000003</v>
+      <c r="E38" t="s">
+        <v>192</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H38" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>196</v>
       </c>
       <c r="D39">
         <v>32372</v>
       </c>
-      <c r="E39">
-        <v>253.40026</v>
+      <c r="E39" t="s">
+        <v>197</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H39" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="C40" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="D40">
         <v>30031</v>
       </c>
-      <c r="E40">
-        <v>116.07216</v>
+      <c r="E40" t="s">
+        <v>202</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H40" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="B41" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="D41">
         <v>17855</v>
       </c>
-      <c r="E41">
-        <v>173.1003</v>
+      <c r="E41" t="s">
+        <v>207</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H41" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="C42" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="D42">
         <v>16235</v>
       </c>
-      <c r="E42">
-        <v>151.126</v>
+      <c r="E42" t="s">
+        <v>212</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="H42" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
       <c r="C43" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="D43">
         <v>17748</v>
       </c>
-      <c r="E43">
-        <v>242.2286</v>
+      <c r="E43" t="s">
+        <v>218</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="H43" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="D44">
         <v>16651</v>
       </c>
-      <c r="E44">
-        <v>89.07</v>
+      <c r="E44" t="s">
+        <v>223</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H44" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="D45">
         <v>15589</v>
       </c>
-      <c r="E45">
-        <v>132.07156000000001</v>
+      <c r="E45" t="s">
+        <v>229</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H45" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>190</v>
+        <v>233</v>
       </c>
       <c r="D46">
         <v>16810</v>
       </c>
-      <c r="E46">
-        <v>144.08225999999999</v>
+      <c r="E46" t="s">
+        <v>234</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H46" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="D47">
         <v>15366</v>
       </c>
-      <c r="E47">
-        <v>60.052</v>
+      <c r="E47" t="s">
+        <v>239</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H47" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="D48">
         <v>16947</v>
       </c>
-      <c r="E48">
-        <v>189.09970000000001</v>
+      <c r="E48" t="s">
+        <v>244</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H48" t="s">
-        <v>199</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" t="s">
         <v>200</v>
       </c>
-      <c r="B49" t="s">
-        <v>163</v>
-      </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>247</v>
       </c>
       <c r="D49">
         <v>18012</v>
       </c>
-      <c r="E49">
-        <v>116.0722</v>
+      <c r="E49" t="s">
+        <v>248</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H49" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>203</v>
+        <v>250</v>
       </c>
       <c r="B50" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="D50">
         <v>17497</v>
       </c>
-      <c r="E50">
-        <v>76.051360000000003</v>
+      <c r="E50" t="s">
+        <v>253</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H50" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="B51" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="C51" t="s">
-        <v>209</v>
+        <v>257</v>
       </c>
       <c r="D51">
         <v>17120</v>
       </c>
-      <c r="E51">
-        <v>115.15034</v>
+      <c r="E51" t="s">
+        <v>258</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H51" t="s">
-        <v>210</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>212</v>
+        <v>261</v>
       </c>
       <c r="C52" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
       <c r="D52">
         <v>15361</v>
       </c>
-      <c r="E52">
-        <v>87.054119999999998</v>
+      <c r="E52" t="s">
+        <v>263</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H52" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="D53">
         <v>15343</v>
       </c>
-      <c r="E53">
-        <v>44.05256</v>
+      <c r="E53" t="s">
+        <v>268</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H53" t="s">
-        <v>219</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="C54" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="D54">
         <v>16199</v>
       </c>
-      <c r="E54">
-        <v>60.055340000000001</v>
+      <c r="E54" t="s">
+        <v>274</v>
       </c>
       <c r="F54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H54" t="s">
-        <v>223</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
       <c r="D55">
         <v>16933</v>
       </c>
-      <c r="E55">
-        <v>396.64836000000003</v>
+      <c r="E55" t="s">
+        <v>181</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H55" t="s">
-        <v>227</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>228</v>
+        <v>280</v>
       </c>
       <c r="B56" t="s">
-        <v>229</v>
+        <v>281</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H56" t="s">
-        <v>231</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>232</v>
+        <v>284</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>233</v>
+        <v>285</v>
       </c>
       <c r="D57">
         <v>28885</v>
@@ -3595,24 +3832,24 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H57" t="s">
-        <v>234</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>287</v>
       </c>
       <c r="B58" t="s">
-        <v>236</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>237</v>
+        <v>289</v>
       </c>
       <c r="D58">
         <v>16718</v>
@@ -3621,50 +3858,50 @@
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G58" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H58" t="s">
-        <v>238</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>291</v>
       </c>
       <c r="B59" t="s">
-        <v>240</v>
+        <v>292</v>
       </c>
       <c r="C59" t="s">
-        <v>241</v>
+        <v>293</v>
       </c>
       <c r="D59">
         <v>8614</v>
       </c>
-      <c r="E59">
-        <v>284.24810100000002</v>
+      <c r="E59" t="s">
+        <v>294</v>
       </c>
       <c r="F59" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G59" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H59" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>243</v>
+        <v>296</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>297</v>
       </c>
       <c r="C60" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
       <c r="D60">
         <v>17721</v>
@@ -3673,24 +3910,24 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G60" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H60" t="s">
-        <v>246</v>
+        <v>299</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>247</v>
+        <v>300</v>
       </c>
       <c r="B61" t="s">
-        <v>248</v>
+        <v>301</v>
       </c>
       <c r="C61" t="s">
-        <v>249</v>
+        <v>302</v>
       </c>
       <c r="D61">
         <v>16388</v>
@@ -3699,50 +3936,50 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G61" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H61" t="s">
-        <v>251</v>
+        <v>304</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>252</v>
+        <v>305</v>
       </c>
       <c r="B62" t="s">
-        <v>253</v>
+        <v>306</v>
       </c>
       <c r="C62" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="D62" t="s">
-        <v>255</v>
+        <v>308</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G62" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H62" t="s">
-        <v>256</v>
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="B63" t="s">
-        <v>258</v>
+        <v>311</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>312</v>
       </c>
       <c r="D63">
         <v>17756</v>
@@ -3751,24 +3988,24 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G63" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H63" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>261</v>
+        <v>314</v>
       </c>
       <c r="B64" t="s">
-        <v>262</v>
+        <v>315</v>
       </c>
       <c r="C64" t="s">
-        <v>263</v>
+        <v>316</v>
       </c>
       <c r="D64">
         <v>32374</v>
@@ -3777,24 +4014,24 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G64" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H64" t="s">
-        <v>264</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="B65" t="s">
-        <v>266</v>
+        <v>319</v>
       </c>
       <c r="C65" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
       <c r="D65">
         <v>50371</v>
@@ -3803,24 +4040,24 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G65" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H65" t="s">
-        <v>268</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>269</v>
+        <v>322</v>
       </c>
       <c r="B66" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="C66" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="D66">
         <v>9009</v>
@@ -3829,24 +4066,24 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G66" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H66" t="s">
-        <v>272</v>
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>273</v>
+        <v>326</v>
       </c>
       <c r="B67" t="s">
-        <v>274</v>
+        <v>327</v>
       </c>
       <c r="C67" t="s">
-        <v>275</v>
+        <v>328</v>
       </c>
       <c r="D67">
         <v>1879</v>
@@ -3855,41 +4092,41 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G67" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H67" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G68" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="H68" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="B69" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="C69" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
       <c r="D69">
         <v>15843</v>
@@ -3898,24 +4135,24 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G69" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H69" t="s">
-        <v>282</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>283</v>
+        <v>336</v>
       </c>
       <c r="B70" t="s">
-        <v>284</v>
+        <v>337</v>
       </c>
       <c r="C70" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="D70">
         <v>28125</v>
@@ -3924,24 +4161,24 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G70" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H70" t="s">
-        <v>286</v>
+        <v>339</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="B71" t="s">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="C71" t="s">
-        <v>289</v>
+        <v>342</v>
       </c>
       <c r="D71">
         <v>28364</v>
@@ -3950,24 +4187,24 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G71" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="H71" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>291</v>
+        <v>344</v>
       </c>
       <c r="B72" t="s">
-        <v>292</v>
+        <v>345</v>
       </c>
       <c r="C72" t="s">
-        <v>293</v>
+        <v>346</v>
       </c>
       <c r="D72">
         <v>31000</v>
@@ -3976,24 +4213,24 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G72" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H72" t="s">
-        <v>294</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>295</v>
+        <v>348</v>
       </c>
       <c r="B73" t="s">
-        <v>296</v>
+        <v>349</v>
       </c>
       <c r="C73" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="D73">
         <v>15600</v>
@@ -4002,24 +4239,24 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G73" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="H73" t="s">
-        <v>299</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>300</v>
+        <v>353</v>
       </c>
       <c r="B74" t="s">
-        <v>301</v>
+        <v>354</v>
       </c>
       <c r="C74" t="s">
-        <v>302</v>
+        <v>355</v>
       </c>
       <c r="D74">
         <v>28088</v>
@@ -4028,24 +4265,24 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G74" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="H74" t="s">
-        <v>303</v>
+        <v>356</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>304</v>
+        <v>357</v>
       </c>
       <c r="B75" t="s">
-        <v>305</v>
+        <v>358</v>
       </c>
       <c r="C75" t="s">
-        <v>306</v>
+        <v>359</v>
       </c>
       <c r="D75">
         <v>28499</v>
@@ -4054,24 +4291,24 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G75" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="H75" t="s">
-        <v>307</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>308</v>
+        <v>361</v>
       </c>
       <c r="B76" t="s">
-        <v>309</v>
+        <v>362</v>
       </c>
       <c r="C76" t="s">
-        <v>310</v>
+        <v>363</v>
       </c>
       <c r="D76">
         <v>17846</v>
@@ -4080,24 +4317,24 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G76" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="H76" t="s">
-        <v>311</v>
+        <v>364</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="B77" t="s">
-        <v>313</v>
+        <v>366</v>
       </c>
       <c r="C77" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
       <c r="D77">
         <v>16243</v>
@@ -4106,24 +4343,24 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G77" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="H77" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>316</v>
+        <v>369</v>
       </c>
       <c r="B78" t="s">
-        <v>317</v>
+        <v>370</v>
       </c>
       <c r="C78" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="D78">
         <v>40968</v>
@@ -4132,24 +4369,24 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G78" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H78" t="s">
-        <v>320</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="B79" t="s">
-        <v>322</v>
+        <v>375</v>
       </c>
       <c r="C79" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="D79">
         <v>8341</v>
@@ -4158,24 +4395,24 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G79" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H79" t="s">
-        <v>324</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>325</v>
+        <v>378</v>
       </c>
       <c r="B80" t="s">
-        <v>326</v>
+        <v>379</v>
       </c>
       <c r="C80" t="s">
-        <v>327</v>
+        <v>380</v>
       </c>
       <c r="D80">
         <v>17579</v>
@@ -4184,24 +4421,24 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G80" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H80" t="s">
-        <v>328</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>329</v>
+        <v>382</v>
       </c>
       <c r="B81" t="s">
-        <v>330</v>
+        <v>383</v>
       </c>
       <c r="C81" t="s">
-        <v>331</v>
+        <v>384</v>
       </c>
       <c r="D81">
         <v>63749</v>
@@ -4210,24 +4447,24 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G81" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H81" t="s">
-        <v>332</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>333</v>
+        <v>386</v>
       </c>
       <c r="B82" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="C82" t="s">
-        <v>334</v>
+        <v>387</v>
       </c>
       <c r="D82">
         <v>16510</v>
@@ -4236,24 +4473,24 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G82" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H82" t="s">
-        <v>335</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>333</v>
+        <v>386</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>334</v>
+        <v>387</v>
       </c>
       <c r="D83">
         <v>16510</v>
@@ -4262,24 +4499,24 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G83" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H83" t="s">
-        <v>336</v>
+        <v>389</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>337</v>
+        <v>390</v>
       </c>
       <c r="B84" t="s">
-        <v>338</v>
+        <v>391</v>
       </c>
       <c r="C84" t="s">
-        <v>339</v>
+        <v>392</v>
       </c>
       <c r="D84">
         <v>30832</v>
@@ -4288,24 +4525,24 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G84" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H84" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>341</v>
+        <v>394</v>
       </c>
       <c r="B85" t="s">
-        <v>342</v>
+        <v>395</v>
       </c>
       <c r="C85" t="s">
-        <v>343</v>
+        <v>396</v>
       </c>
       <c r="D85">
         <v>16508</v>
@@ -4314,24 +4551,24 @@
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G85" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H85" t="s">
-        <v>344</v>
+        <v>397</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>345</v>
+        <v>398</v>
       </c>
       <c r="B86" t="s">
-        <v>346</v>
+        <v>399</v>
       </c>
       <c r="C86" t="s">
-        <v>347</v>
+        <v>400</v>
       </c>
       <c r="D86">
         <v>17240</v>
@@ -4340,24 +4577,24 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G86" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="H86" t="s">
-        <v>348</v>
+        <v>401</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>349</v>
+        <v>402</v>
       </c>
       <c r="B87" t="s">
-        <v>350</v>
+        <v>403</v>
       </c>
       <c r="C87" t="s">
-        <v>351</v>
+        <v>404</v>
       </c>
       <c r="D87">
         <v>18153</v>
@@ -4366,24 +4603,24 @@
         <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G87" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H87" t="s">
-        <v>352</v>
+        <v>405</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
       <c r="B88" t="s">
-        <v>354</v>
+        <v>407</v>
       </c>
       <c r="C88" t="s">
-        <v>355</v>
+        <v>408</v>
       </c>
       <c r="D88">
         <v>514</v>
@@ -4392,24 +4629,24 @@
         <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G88" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H88" t="s">
-        <v>356</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>357</v>
+        <v>410</v>
       </c>
       <c r="B89" t="s">
-        <v>358</v>
+        <v>411</v>
       </c>
       <c r="C89" t="s">
-        <v>359</v>
+        <v>412</v>
       </c>
       <c r="D89">
         <v>5391</v>
@@ -4418,38 +4655,38 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G89" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="H89" t="s">
-        <v>361</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>362</v>
+        <v>415</v>
       </c>
       <c r="E90">
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G90" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="H90" t="s">
-        <v>363</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>364</v>
+        <v>417</v>
       </c>
       <c r="C91" t="s">
-        <v>365</v>
+        <v>418</v>
       </c>
       <c r="D91">
         <v>5656</v>
@@ -4458,70 +4695,70 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G91" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="H91" t="s">
-        <v>366</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="C92" t="s">
-        <v>368</v>
+        <v>421</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G92" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="H92" t="s">
-        <v>369</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>370</v>
+        <v>423</v>
       </c>
       <c r="B93" t="s">
-        <v>371</v>
+        <v>424</v>
       </c>
       <c r="C93" t="s">
-        <v>372</v>
+        <v>425</v>
       </c>
       <c r="D93" t="s">
-        <v>371</v>
+        <v>424</v>
       </c>
       <c r="E93">
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G93" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="H93" t="s">
-        <v>373</v>
+        <v>426</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>374</v>
+        <v>427</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>428</v>
       </c>
       <c r="C94" t="s">
-        <v>376</v>
+        <v>429</v>
       </c>
       <c r="D94">
         <v>27881</v>
@@ -4530,24 +4767,24 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G94" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="H94" t="s">
-        <v>377</v>
+        <v>430</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>378</v>
+        <v>431</v>
       </c>
       <c r="B95" t="s">
-        <v>379</v>
+        <v>432</v>
       </c>
       <c r="C95" t="s">
-        <v>380</v>
+        <v>433</v>
       </c>
       <c r="D95">
         <v>10280</v>
@@ -4556,24 +4793,24 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G95" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H95" t="s">
-        <v>381</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>382</v>
+        <v>435</v>
       </c>
       <c r="B96" t="s">
-        <v>379</v>
+        <v>432</v>
       </c>
       <c r="C96" t="s">
-        <v>383</v>
+        <v>436</v>
       </c>
       <c r="D96">
         <v>52026</v>
@@ -4582,24 +4819,24 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G96" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H96" t="s">
-        <v>384</v>
+        <v>437</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>385</v>
+        <v>438</v>
       </c>
       <c r="B97" t="s">
-        <v>386</v>
+        <v>439</v>
       </c>
       <c r="C97" t="s">
-        <v>387</v>
+        <v>440</v>
       </c>
       <c r="D97">
         <v>17447</v>
@@ -4608,24 +4845,24 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G97" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H97" t="s">
-        <v>388</v>
+        <v>441</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>389</v>
+        <v>442</v>
       </c>
       <c r="B98" t="s">
-        <v>390</v>
+        <v>443</v>
       </c>
       <c r="C98" t="s">
-        <v>391</v>
+        <v>444</v>
       </c>
       <c r="D98">
         <v>15384</v>
@@ -4634,24 +4871,24 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G98" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H98" t="s">
-        <v>392</v>
+        <v>445</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>393</v>
+        <v>446</v>
       </c>
       <c r="B99" t="s">
-        <v>386</v>
+        <v>439</v>
       </c>
       <c r="C99" t="s">
-        <v>394</v>
+        <v>447</v>
       </c>
       <c r="D99">
         <v>17580</v>
@@ -4660,24 +4897,24 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G99" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H99" t="s">
-        <v>395</v>
+        <v>448</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>396</v>
+        <v>449</v>
       </c>
       <c r="B100" t="s">
-        <v>397</v>
+        <v>450</v>
       </c>
       <c r="C100" t="s">
-        <v>398</v>
+        <v>451</v>
       </c>
       <c r="D100">
         <v>6570</v>
@@ -4686,24 +4923,24 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G100" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H100" t="s">
-        <v>399</v>
+        <v>452</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>400</v>
+        <v>453</v>
       </c>
       <c r="B101" t="s">
-        <v>401</v>
+        <v>454</v>
       </c>
       <c r="C101" t="s">
-        <v>402</v>
+        <v>455</v>
       </c>
       <c r="D101">
         <v>37659</v>
@@ -4712,24 +4949,24 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G101" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H101" t="s">
-        <v>403</v>
+        <v>456</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>404</v>
+        <v>457</v>
       </c>
       <c r="B102" t="s">
-        <v>405</v>
+        <v>458</v>
       </c>
       <c r="C102" t="s">
-        <v>406</v>
+        <v>459</v>
       </c>
       <c r="D102">
         <v>7940</v>
@@ -4738,24 +4975,24 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G102" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H102" t="s">
-        <v>407</v>
+        <v>460</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>408</v>
+        <v>461</v>
       </c>
       <c r="B103" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="C103" t="s">
-        <v>410</v>
+        <v>463</v>
       </c>
       <c r="D103">
         <v>75950</v>
@@ -4764,47 +5001,47 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G103" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H103" t="s">
-        <v>411</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>412</v>
+        <v>465</v>
       </c>
       <c r="B104" t="s">
-        <v>379</v>
+        <v>432</v>
       </c>
       <c r="C104" t="s">
-        <v>413</v>
+        <v>466</v>
       </c>
       <c r="E104">
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G104" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H104" t="s">
-        <v>414</v>
+        <v>467</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>415</v>
+        <v>468</v>
       </c>
       <c r="B105" t="s">
-        <v>397</v>
+        <v>450</v>
       </c>
       <c r="C105" t="s">
-        <v>416</v>
+        <v>469</v>
       </c>
       <c r="D105">
         <v>10352</v>
@@ -4813,24 +5050,24 @@
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G105" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H105" t="s">
-        <v>417</v>
+        <v>470</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>418</v>
+        <v>471</v>
       </c>
       <c r="B106" t="s">
-        <v>419</v>
+        <v>472</v>
       </c>
       <c r="C106" t="s">
-        <v>420</v>
+        <v>473</v>
       </c>
       <c r="D106">
         <v>32325</v>
@@ -4839,13 +5076,173 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>230</v>
+        <v>282</v>
       </c>
       <c r="G106" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="H106" t="s">
-        <v>421</v>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>475</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107" t="s">
+        <v>282</v>
+      </c>
+      <c r="G107" t="s">
+        <v>269</v>
+      </c>
+      <c r="H107" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>477</v>
+      </c>
+      <c r="G108" t="s">
+        <v>224</v>
+      </c>
+      <c r="H108" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>479</v>
+      </c>
+      <c r="G109" t="s">
+        <v>39</v>
+      </c>
+      <c r="H109" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>481</v>
+      </c>
+      <c r="G110" t="s">
+        <v>55</v>
+      </c>
+      <c r="H110" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>483</v>
+      </c>
+      <c r="G111" t="s">
+        <v>372</v>
+      </c>
+      <c r="H111" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>485</v>
+      </c>
+      <c r="G112" t="s">
+        <v>372</v>
+      </c>
+      <c r="H112" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>487</v>
+      </c>
+      <c r="G113" t="s">
+        <v>372</v>
+      </c>
+      <c r="H113" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>489</v>
+      </c>
+      <c r="G114" t="s">
+        <v>372</v>
+      </c>
+      <c r="H114" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>491</v>
+      </c>
+      <c r="G115" t="s">
+        <v>269</v>
+      </c>
+      <c r="H115" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>493</v>
+      </c>
+      <c r="G116" t="s">
+        <v>372</v>
+      </c>
+      <c r="H116" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>199</v>
+      </c>
+      <c r="G117" t="s">
+        <v>224</v>
+      </c>
+      <c r="H117" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>496</v>
+      </c>
+      <c r="G118" t="s">
+        <v>372</v>
+      </c>
+      <c r="H118" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>498</v>
+      </c>
+      <c r="G119" t="s">
+        <v>269</v>
+      </c>
+      <c r="H119" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>500</v>
+      </c>
+      <c r="G120" t="s">
+        <v>372</v>
+      </c>
+      <c r="H120" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>